<commit_message>
isa and assembler fixed
</commit_message>
<xml_diff>
--- a/isa.xlsx
+++ b/isa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEF8D55-BEF5-49C0-9ED2-A06FAEFD3FED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE143125-5CAA-434C-B23E-79BB6554DEA3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +129,14 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -425,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -484,28 +491,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -791,7 +807,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,12 +816,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -885,24 +901,24 @@
       <c r="E3" s="10">
         <v>0</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="22" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="22" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="25"/>
       <c r="R3" s="1">
         <v>0</v>
       </c>
@@ -923,24 +939,24 @@
       <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="22" t="s">
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="22" t="s">
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
       <c r="R4" s="1">
         <v>1</v>
       </c>
@@ -961,24 +977,24 @@
       <c r="E5" s="10">
         <v>0</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="22" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="22" t="s">
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="25"/>
       <c r="R5" s="1">
         <v>2</v>
       </c>
@@ -999,24 +1015,24 @@
       <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="22" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="22" t="s">
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
       <c r="R6" s="1">
         <v>3</v>
       </c>
@@ -1037,24 +1053,22 @@
       <c r="E7" s="10">
         <v>0</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="16">
-        <v>0</v>
-      </c>
-      <c r="K7" s="25" t="s">
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="30"/>
       <c r="R7" s="1">
         <v>4</v>
       </c>
@@ -1075,24 +1089,22 @@
       <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="16">
-        <v>0</v>
-      </c>
-      <c r="K8" s="25" t="s">
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="27"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="30"/>
       <c r="R8" s="1">
         <v>5</v>
       </c>
@@ -1125,18 +1137,18 @@
       <c r="I9" s="16">
         <v>0</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="22" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
       <c r="R9" s="1">
         <v>6</v>
       </c>
@@ -1169,16 +1181,16 @@
       <c r="I10" s="16">
         <v>0</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="27"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="22"/>
       <c r="R10" s="17">
         <v>7</v>
       </c>
@@ -1211,18 +1223,16 @@
       <c r="I11" s="16">
         <v>0</v>
       </c>
-      <c r="J11" s="16">
-        <v>0</v>
-      </c>
-      <c r="K11" s="25" t="s">
+      <c r="J11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="27"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="22"/>
       <c r="R11" s="17">
         <v>8</v>
       </c>
@@ -1255,18 +1265,16 @@
       <c r="I12" s="16">
         <v>0</v>
       </c>
-      <c r="J12" s="16">
-        <v>0</v>
-      </c>
-      <c r="K12" s="25" t="s">
+      <c r="J12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="27"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="22"/>
       <c r="R12" s="17">
         <v>9</v>
       </c>
@@ -1299,18 +1307,16 @@
       <c r="I13" s="16">
         <v>0</v>
       </c>
-      <c r="J13" s="16">
-        <v>0</v>
-      </c>
-      <c r="K13" s="25" t="s">
+      <c r="J13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="27"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="22"/>
       <c r="R13" s="17">
         <v>10</v>
       </c>
@@ -1343,18 +1349,16 @@
       <c r="I14" s="16">
         <v>0</v>
       </c>
-      <c r="J14" s="16">
-        <v>0</v>
-      </c>
-      <c r="K14" s="25" t="s">
+      <c r="J14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="27"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="22"/>
       <c r="R14" s="17">
         <v>11</v>
       </c>
@@ -1387,18 +1391,16 @@
       <c r="I15" s="16">
         <v>0</v>
       </c>
-      <c r="J15" s="16">
-        <v>0</v>
-      </c>
-      <c r="K15" s="25" t="s">
+      <c r="J15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="27"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="22"/>
       <c r="R15" s="17">
         <v>12</v>
       </c>
@@ -1409,14 +1411,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="K13:Q13"/>
-    <mergeCell ref="K14:Q14"/>
-    <mergeCell ref="K15:Q15"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="K11:Q11"/>
-    <mergeCell ref="K12:Q12"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="F4:I4"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="F6:I6"/>
@@ -1427,13 +1426,16 @@
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="K8:Q8"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="J8:Q8"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="J11:Q11"/>
+    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="J13:Q13"/>
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="J15:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
addresses extended to 12 bit
</commit_message>
<xml_diff>
--- a/isa.xlsx
+++ b/isa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE143125-5CAA-434C-B23E-79BB6554DEA3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7E1298-68E6-4557-99DD-EDACBB202D46}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,6 +491,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,30 +522,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -807,7 +807,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,12 +816,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -901,24 +901,24 @@
       <c r="E3" s="10">
         <v>0</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="23" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="23" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="25"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
       <c r="R3" s="1">
         <v>0</v>
       </c>
@@ -939,24 +939,24 @@
       <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="23" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="23" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
       <c r="R4" s="1">
         <v>1</v>
       </c>
@@ -977,24 +977,24 @@
       <c r="E5" s="10">
         <v>0</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="23" t="s">
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="23" t="s">
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="25"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
       <c r="R5" s="1">
         <v>2</v>
       </c>
@@ -1015,24 +1015,24 @@
       <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="23" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="23" t="s">
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="25"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="24"/>
       <c r="R6" s="1">
         <v>3</v>
       </c>
@@ -1053,22 +1053,22 @@
       <c r="E7" s="10">
         <v>0</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="28" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="27"/>
       <c r="R7" s="1">
         <v>4</v>
       </c>
@@ -1089,22 +1089,22 @@
       <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="28" t="s">
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="30"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="27"/>
       <c r="R8" s="1">
         <v>5</v>
       </c>
@@ -1137,18 +1137,18 @@
       <c r="I9" s="16">
         <v>0</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="23" t="s">
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="25"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="24"/>
       <c r="R9" s="1">
         <v>6</v>
       </c>
@@ -1169,28 +1169,20 @@
       <c r="E10" s="10">
         <v>1</v>
       </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
-      <c r="H10" s="16">
-        <v>0</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0</v>
-      </c>
-      <c r="J10" s="20" t="s">
+      <c r="F10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="30"/>
       <c r="R10" s="17">
         <v>7</v>
       </c>
@@ -1211,28 +1203,20 @@
       <c r="E11" s="10">
         <v>0</v>
       </c>
-      <c r="F11" s="18">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0</v>
-      </c>
-      <c r="J11" s="20" t="s">
+      <c r="F11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="22"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="30"/>
       <c r="R11" s="17">
         <v>8</v>
       </c>
@@ -1253,28 +1237,20 @@
       <c r="E12" s="10">
         <v>1</v>
       </c>
-      <c r="F12" s="18">
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0</v>
-      </c>
-      <c r="I12" s="16">
-        <v>0</v>
-      </c>
-      <c r="J12" s="20" t="s">
+      <c r="F12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="22"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="30"/>
       <c r="R12" s="17">
         <v>9</v>
       </c>
@@ -1295,28 +1271,20 @@
       <c r="E13" s="10">
         <v>0</v>
       </c>
-      <c r="F13" s="18">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="16">
-        <v>0</v>
-      </c>
-      <c r="I13" s="16">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20" t="s">
+      <c r="F13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="22"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="30"/>
       <c r="R13" s="17">
         <v>10</v>
       </c>
@@ -1337,28 +1305,20 @@
       <c r="E14" s="10">
         <v>1</v>
       </c>
-      <c r="F14" s="18">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="16">
-        <v>0</v>
-      </c>
-      <c r="I14" s="16">
-        <v>0</v>
-      </c>
-      <c r="J14" s="20" t="s">
+      <c r="F14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="22"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="30"/>
       <c r="R14" s="17">
         <v>11</v>
       </c>
@@ -1379,28 +1339,20 @@
       <c r="E15" s="13">
         <v>0</v>
       </c>
-      <c r="F15" s="18">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0</v>
-      </c>
-      <c r="I15" s="16">
-        <v>0</v>
-      </c>
-      <c r="J15" s="20" t="s">
+      <c r="F15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="22"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="30"/>
       <c r="R15" s="17">
         <v>12</v>
       </c>
@@ -1411,11 +1363,14 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F10:Q10"/>
+    <mergeCell ref="F11:Q11"/>
+    <mergeCell ref="F12:Q12"/>
+    <mergeCell ref="F13:Q13"/>
+    <mergeCell ref="F14:Q14"/>
+    <mergeCell ref="F15:Q15"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="F6:I6"/>
@@ -1428,14 +1383,11 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="J7:Q7"/>
     <mergeCell ref="J8:Q8"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="J11:Q11"/>
-    <mergeCell ref="J12:Q12"/>
-    <mergeCell ref="J13:Q13"/>
-    <mergeCell ref="J14:Q14"/>
-    <mergeCell ref="J15:Q15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>